<commit_message>
has_text improved as it was given too many false negatives
</commit_message>
<xml_diff>
--- a/outputs/results/recording1/summary.xlsx
+++ b/outputs/results/recording1/summary.xlsx
@@ -167,7 +167,7 @@
     <from>
       <col>22</col>
       <colOff>0</colOff>
-      <row>0</row>
+      <row>20</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="14287500" cy="9525000"/>
@@ -178,31 +178,6 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>22</col>
-      <colOff>0</colOff>
-      <row>20</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="14287500" cy="9525000"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="3" name="Image 3" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -505,7 +480,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -543,7 +518,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>tests .</t>
+          <t>Dead .</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -562,7 +537,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>test is</t>
+          <t>alive .</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -581,7 +556,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>test B .</t>
+          <t>test A</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -600,7 +575,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>tost B .</t>
+          <t>test B .</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -613,215 +588,6 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>tost is .</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>tost is</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>test is</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>test 3 .</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>test is .</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" t="n">
-        <v>1</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>test B .</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>0</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>test a</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Test is</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>1</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" t="n">
-        <v>1</v>
-      </c>
-      <c r="E13" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>tast is</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C14" t="n">
-        <v>0</v>
-      </c>
-      <c r="D14" t="n">
-        <v>0</v>
-      </c>
-      <c r="E14" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>tests .</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>0</v>
-      </c>
-      <c r="C15" t="n">
-        <v>0</v>
-      </c>
-      <c r="D15" t="n">
-        <v>0</v>
-      </c>
-      <c r="E15" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>test is</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>0</v>
-      </c>
-      <c r="C16" t="n">
-        <v>0</v>
-      </c>
-      <c r="D16" t="n">
-        <v>0</v>
-      </c>
-      <c r="E16" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
mite detector confidence increased and check alive thershold set
</commit_message>
<xml_diff>
--- a/outputs/results/recording1/summary.xlsx
+++ b/outputs/results/recording1/summary.xlsx
@@ -518,17 +518,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Dead .</t>
+          <t>tests :</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -537,55 +537,55 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>alive .</t>
+          <t>venom 1 .</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>11.11</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>test A</t>
+          <t>tests like</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>test B .</t>
+          <t>tost is</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>

</xml_diff>